<commit_message>
Ajusta ponto médio questão 1
</commit_message>
<xml_diff>
--- a/Arquivos/Estatistica/Prova 01.xlsx
+++ b/Arquivos/Estatistica/Prova 01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faculdade\05 - Estatística\Atividades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faculdade\AtividadesFaculdade\Arquivos\Estatistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91DFD3B-C4CE-4343-AEAB-C6256412B4C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7915854B-5480-405B-BB72-1E2763A082B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{A77F4E86-F905-4AA5-9E5C-6D71E79B919B}"/>
   </bookViews>
@@ -254,12 +254,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="168" formatCode="0.00000"/>
-    <numFmt numFmtId="175" formatCode="0.0000000000"/>
-    <numFmt numFmtId="176" formatCode="0.0"/>
-    <numFmt numFmtId="177" formatCode="0.00000000000"/>
-    <numFmt numFmtId="179" formatCode="0.000000000000"/>
-    <numFmt numFmtId="180" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.00000000000"/>
+    <numFmt numFmtId="168" formatCode="0.000000000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -417,28 +417,28 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499F8018-6712-43CD-84EC-58B58B271E58}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:I26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +883,7 @@
       <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="6">
         <f>15.9-14</f>
         <v>1.9000000000000004</v>
       </c>
@@ -1038,8 +1038,8 @@
       <c r="E20" s="3">
         <v>9</v>
       </c>
-      <c r="F20" s="10">
-        <v>225</v>
+      <c r="F20" s="6">
+        <v>14.16</v>
       </c>
       <c r="G20" s="10">
         <f>(E20/25)*100</f>
@@ -1066,8 +1066,8 @@
       <c r="E21" s="3">
         <v>4</v>
       </c>
-      <c r="F21" s="10">
-        <v>227</v>
+      <c r="F21" s="6">
+        <v>14.48</v>
       </c>
       <c r="G21" s="10">
         <f t="shared" ref="G21:G26" si="0">(E21/25)*100</f>
@@ -1095,8 +1095,8 @@
       <c r="E22" s="3">
         <v>4</v>
       </c>
-      <c r="F22" s="10">
-        <v>229</v>
+      <c r="F22" s="6">
+        <v>14.8</v>
       </c>
       <c r="G22" s="10">
         <f t="shared" si="0"/>
@@ -1124,8 +1124,8 @@
       <c r="E23" s="3">
         <v>3</v>
       </c>
-      <c r="F23" s="10">
-        <v>231</v>
+      <c r="F23" s="6">
+        <v>15.12</v>
       </c>
       <c r="G23" s="10">
         <f t="shared" si="0"/>
@@ -1153,8 +1153,8 @@
       <c r="E24" s="3">
         <v>0</v>
       </c>
-      <c r="F24" s="10">
-        <v>233</v>
+      <c r="F24" s="6">
+        <v>15.44</v>
       </c>
       <c r="G24" s="10">
         <f t="shared" si="0"/>
@@ -1182,8 +1182,8 @@
       <c r="E25" s="3">
         <v>5</v>
       </c>
-      <c r="F25" s="10">
-        <v>235</v>
+      <c r="F25" s="6">
+        <v>15.76</v>
       </c>
       <c r="G25" s="10">
         <f t="shared" si="0"/>
@@ -1565,7 +1565,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="14">
-        <f t="shared" ref="B14:B17" si="0">((A3-$B$9)^2)*B3</f>
+        <f t="shared" ref="B14:B15" si="0">((A3-$B$9)^2)*B3</f>
         <v>41606.666666666606</v>
       </c>
       <c r="C14" t="s">

</xml_diff>